<commit_message>
eliminar cosas que no se usaban
</commit_message>
<xml_diff>
--- a/media/excel/image.xlsx
+++ b/media/excel/image.xlsx
@@ -73,14 +73,14 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="blob_Q0DXKAR.jpg"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="blob_wpRytrB.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -94,7 +94,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="19126200" cy="9525000"/>
+          <a:ext cx="19011900" cy="8810625"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>